<commit_message>
Correction description DocumentReference 03d302022e9a3c33c34611bd5146e552e1984459
</commit_message>
<xml_diff>
--- a/298-Ajout-de-l'évènement/ig/StructureDefinition-tddui-document-reference.xlsx
+++ b/298-Ajout-de-l'évènement/ig/StructureDefinition-tddui-document-reference.xlsx
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-10-14T09:28:59+00:00</t>
+    <t>2025-10-15T10:12:33+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -84,7 +84,7 @@
     <t>Description</t>
   </si>
   <si>
-    <t>Profil de la ressource TDDUIDocumentReference pour les pièces jointes liées à l’événement et à l'évaluation.</t>
+    <t>Profil de la ressource SimplifiedPublishDocumentReference pour les pièces jointes liées à l’événement et à l'évaluation.</t>
   </si>
   <si>
     <t>Purpose</t>

</xml_diff>